<commit_message>
KIBON-165: Benutzerverwaltung: Bei den Gemeinde Rollen kann die Gemeinde bearbeitet werden. Neue Spalte im Benutzer-Report
</commit_message>
<xml_diff>
--- a/ebegu-server/src/main/resources/reporting/Benutzer.xlsx
+++ b/ebegu-server/src/main/resources/reporting/Benutzer.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20829"/>
   <workbookPr/>
+  <xr:revisionPtr revIDLastSave="3" documentId="11_80BED6E07095660F07BF7CE8808D0197A6985912" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{B6C82381-52D1-4A2F-9D62-B766F5AADA47}"/>
   <bookViews>
-    <workbookView xWindow="975" yWindow="360" windowWidth="28800" windowHeight="12435"/>
+    <workbookView xWindow="975" yWindow="360" windowWidth="28800" windowHeight="12435" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="125725"/>
+  <calcPr calcId="179020"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -19,26 +20,74 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="38">
+  <si>
+    <t>Benutzer</t>
+  </si>
+  <si>
+    <t>Stichtag</t>
+  </si>
+  <si>
+    <t>{stichtag}</t>
+  </si>
+  <si>
+    <t>Username</t>
+  </si>
   <si>
     <t>Vorname</t>
   </si>
   <si>
+    <t>Nachname</t>
+  </si>
+  <si>
+    <t>E-Mail</t>
+  </si>
+  <si>
+    <t>Rolle</t>
+  </si>
+  <si>
+    <t>Rolle gültig bis</t>
+  </si>
+  <si>
+    <t>Gemeinde(n)</t>
+  </si>
+  <si>
+    <t>Institution</t>
+  </si>
+  <si>
+    <t>Trägerschaft</t>
+  </si>
+  <si>
+    <t>Kita</t>
+  </si>
+  <si>
+    <t>Tagesfamilien</t>
+  </si>
+  <si>
+    <t>Tagi</t>
+  </si>
+  <si>
+    <t>Tagesschulen</t>
+  </si>
+  <si>
+    <t>Ferieninsel</t>
+  </si>
+  <si>
+    <t>Jugendamt-Angebote</t>
+  </si>
+  <si>
+    <t>Schulamt-Angebote</t>
+  </si>
+  <si>
+    <t>Gesperrt</t>
+  </si>
+  <si>
+    <t>{username}</t>
+  </si>
+  <si>
     <t>{vorname}</t>
   </si>
   <si>
-    <t>Benutzer</t>
-  </si>
-  <si>
-    <t>Stichtag</t>
-  </si>
-  <si>
-    <t>{stichtag}</t>
-  </si>
-  <si>
-    <t>{username}</t>
-  </si>
-  <si>
     <t>{nachname}</t>
   </si>
   <si>
@@ -48,92 +97,50 @@
     <t>{role}</t>
   </si>
   <si>
+    <t>{roleGueltigBis}</t>
+  </si>
+  <si>
+    <t>{gemeinden}</t>
+  </si>
+  <si>
     <t>{institution}</t>
   </si>
   <si>
     <t>{traegerschaft}</t>
   </si>
   <si>
+    <t>{isKita}</t>
+  </si>
+  <si>
+    <t>{isTagesfamilien}</t>
+  </si>
+  <si>
+    <t>{isTagi}</t>
+  </si>
+  <si>
+    <t>{isTagesschule}</t>
+  </si>
+  <si>
+    <t>{isFerieninsel}</t>
+  </si>
+  <si>
+    <t>{isJugendamt}</t>
+  </si>
+  <si>
+    <t>{isSchulamt}</t>
+  </si>
+  <si>
     <t>{gesperrt}</t>
   </si>
   <si>
     <t>{repeatBenutzerRow}</t>
-  </si>
-  <si>
-    <t>Gesperrt</t>
-  </si>
-  <si>
-    <t>Username</t>
-  </si>
-  <si>
-    <t>Nachname</t>
-  </si>
-  <si>
-    <t>E-Mail</t>
-  </si>
-  <si>
-    <t>Rolle</t>
-  </si>
-  <si>
-    <t>Institution</t>
-  </si>
-  <si>
-    <t>Trägerschaft</t>
-  </si>
-  <si>
-    <t>Rolle gültig bis</t>
-  </si>
-  <si>
-    <t>{roleGueltigBis}</t>
-  </si>
-  <si>
-    <t>Kita</t>
-  </si>
-  <si>
-    <t>Tagi</t>
-  </si>
-  <si>
-    <t>Tagesschulen</t>
-  </si>
-  <si>
-    <t>Ferieninsel</t>
-  </si>
-  <si>
-    <t>Jugendamt-Angebote</t>
-  </si>
-  <si>
-    <t>Schulamt-Angebote</t>
-  </si>
-  <si>
-    <t>{isKita}</t>
-  </si>
-  <si>
-    <t>{isTagi}</t>
-  </si>
-  <si>
-    <t>{isTagesschule}</t>
-  </si>
-  <si>
-    <t>{isFerieninsel}</t>
-  </si>
-  <si>
-    <t>{isJugendamt}</t>
-  </si>
-  <si>
-    <t>{isSchulamt}</t>
-  </si>
-  <si>
-    <t>{isTagesfamilien}</t>
-  </si>
-  <si>
-    <t>Tagesfamilien</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -238,11 +245,11 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -272,7 +279,7 @@
     </dxf>
   </dxfs>
   <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
-    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2">
+    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2" xr9:uid="{00000000-0011-0000-FFFF-FFFF00000000}">
       <tableStyleElement type="wholeTable" dxfId="1"/>
       <tableStyleElement type="headerRow" dxfId="0"/>
     </tableStyle>
@@ -543,43 +550,43 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q15"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:R15"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="J6" sqref="J6"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0" xr3:uid="{AEA406A1-0E4B-5B11-9CD5-51D6E497D94C}">
+      <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="22.28515625" customWidth="1"/>
     <col min="2" max="2" width="22" customWidth="1"/>
     <col min="3" max="3" width="21" customWidth="1"/>
     <col min="4" max="4" width="36" customWidth="1"/>
     <col min="5" max="5" width="33.7109375" customWidth="1"/>
-    <col min="6" max="6" width="16.5703125" customWidth="1"/>
-    <col min="7" max="7" width="30.140625" customWidth="1"/>
-    <col min="8" max="8" width="28.7109375" customWidth="1"/>
-    <col min="9" max="9" width="7.28515625" customWidth="1"/>
-    <col min="10" max="10" width="16.42578125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="7.42578125" customWidth="1"/>
-    <col min="12" max="12" width="14.5703125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="13.85546875" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="20.28515625" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="18.7109375" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="12.28515625" customWidth="1"/>
+    <col min="6" max="7" width="16.5703125" customWidth="1"/>
+    <col min="8" max="8" width="30.140625" customWidth="1"/>
+    <col min="9" max="9" width="28.7109375" customWidth="1"/>
+    <col min="10" max="10" width="7.28515625" customWidth="1"/>
+    <col min="11" max="11" width="16.42578125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="7.42578125" customWidth="1"/>
+    <col min="13" max="13" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="20.28515625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="18.7109375" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="12.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" ht="21" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:18" ht="21">
       <c r="A1" s="1" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="B1" s="1"/>
       <c r="C1" s="2"/>
@@ -595,8 +602,9 @@
       <c r="M1" s="2"/>
       <c r="N1" s="2"/>
       <c r="O1" s="2"/>
-    </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="P1" s="2"/>
+    </row>
+    <row r="2" spans="1:18">
       <c r="C2" s="3"/>
       <c r="D2" s="3"/>
       <c r="E2" s="3"/>
@@ -610,13 +618,14 @@
       <c r="M2" s="3"/>
       <c r="N2" s="3"/>
       <c r="O2" s="3"/>
-    </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="P2" s="3"/>
+    </row>
+    <row r="3" spans="1:18">
       <c r="A3" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C3" s="5"/>
       <c r="D3" s="5"/>
@@ -631,8 +640,9 @@
       <c r="M3" s="5"/>
       <c r="N3" s="5"/>
       <c r="O3" s="5"/>
-    </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="P3" s="5"/>
+    </row>
+    <row r="4" spans="1:18">
       <c r="C4" s="3"/>
       <c r="D4" s="3"/>
       <c r="E4" s="3"/>
@@ -646,111 +656,118 @@
       <c r="M4" s="3"/>
       <c r="N4" s="3"/>
       <c r="O4" s="3"/>
-    </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="P4" s="3"/>
+    </row>
+    <row r="5" spans="1:18">
       <c r="A5" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="C5" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="D5" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="E5" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="F5" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="G5" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="H5" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="I5" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="J5" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="K5" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="L5" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="B5" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="C5" s="8" t="s">
+      <c r="M5" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="D5" s="8" t="s">
+      <c r="N5" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="E5" s="8" t="s">
+      <c r="O5" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="F5" s="8" t="s">
+      <c r="P5" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="Q5" s="7" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="6" spans="1:18">
+      <c r="A6" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="G5" s="8" t="s">
-        <v>18</v>
-      </c>
-      <c r="H5" s="8" t="s">
-        <v>19</v>
-      </c>
-      <c r="I5" s="8" t="s">
+      <c r="B6" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="C6" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="J5" s="8" t="s">
+      <c r="D6" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="E6" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="F6" s="11" t="s">
+        <v>25</v>
+      </c>
+      <c r="G6" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="H6" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="I6" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="J6" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="K6" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="L6" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="M6" s="10" t="s">
+        <v>32</v>
+      </c>
+      <c r="N6" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="O6" s="10" t="s">
+        <v>34</v>
+      </c>
+      <c r="P6" s="10" t="s">
         <v>35</v>
       </c>
-      <c r="K5" s="8" t="s">
-        <v>23</v>
-      </c>
-      <c r="L5" s="8" t="s">
-        <v>24</v>
-      </c>
-      <c r="M5" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="N5" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="O5" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="P5" s="7" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A6" s="9" t="s">
-        <v>5</v>
-      </c>
-      <c r="B6" s="9" t="s">
-        <v>1</v>
-      </c>
-      <c r="C6" s="9" t="s">
-        <v>6</v>
-      </c>
-      <c r="D6" s="9" t="s">
-        <v>7</v>
-      </c>
-      <c r="E6" s="9" t="s">
-        <v>8</v>
-      </c>
-      <c r="F6" s="11" t="s">
-        <v>21</v>
-      </c>
-      <c r="G6" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="H6" s="9" t="s">
-        <v>10</v>
-      </c>
-      <c r="I6" s="10" t="s">
-        <v>28</v>
-      </c>
-      <c r="J6" s="10" t="s">
-        <v>34</v>
-      </c>
-      <c r="K6" s="10" t="s">
-        <v>29</v>
-      </c>
-      <c r="L6" s="10" t="s">
-        <v>30</v>
-      </c>
-      <c r="M6" s="10" t="s">
-        <v>31</v>
-      </c>
-      <c r="N6" s="10" t="s">
-        <v>32</v>
-      </c>
-      <c r="O6" s="10" t="s">
-        <v>33</v>
-      </c>
-      <c r="P6" s="10" t="s">
-        <v>11</v>
-      </c>
-      <c r="Q6" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="Q6" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="R6" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="7" spans="1:18">
       <c r="C7" s="3"/>
       <c r="D7" s="3"/>
       <c r="E7" s="3"/>
@@ -764,8 +781,9 @@
       <c r="M7" s="3"/>
       <c r="N7" s="3"/>
       <c r="O7" s="3"/>
-    </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="P7" s="3"/>
+    </row>
+    <row r="8" spans="1:18">
       <c r="A8" s="4"/>
       <c r="B8" s="4"/>
       <c r="C8" s="5"/>
@@ -781,8 +799,9 @@
       <c r="M8" s="5"/>
       <c r="N8" s="5"/>
       <c r="O8" s="5"/>
-    </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="P8" s="5"/>
+    </row>
+    <row r="9" spans="1:18">
       <c r="C9" s="3"/>
       <c r="D9" s="3"/>
       <c r="E9" s="3"/>
@@ -796,8 +815,9 @@
       <c r="M9" s="3"/>
       <c r="N9" s="3"/>
       <c r="O9" s="3"/>
-    </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="P9" s="3"/>
+    </row>
+    <row r="10" spans="1:18">
       <c r="C10" s="3"/>
       <c r="D10" s="3"/>
       <c r="E10" s="3"/>
@@ -811,8 +831,9 @@
       <c r="M10" s="3"/>
       <c r="N10" s="3"/>
       <c r="O10" s="3"/>
-    </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="P10" s="3"/>
+    </row>
+    <row r="11" spans="1:18">
       <c r="C11" s="3"/>
       <c r="D11" s="3"/>
       <c r="E11" s="3"/>
@@ -826,8 +847,9 @@
       <c r="M11" s="3"/>
       <c r="N11" s="3"/>
       <c r="O11" s="3"/>
-    </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="P11" s="3"/>
+    </row>
+    <row r="12" spans="1:18">
       <c r="C12" s="3"/>
       <c r="D12" s="3"/>
       <c r="E12" s="3"/>
@@ -841,8 +863,9 @@
       <c r="M12" s="3"/>
       <c r="N12" s="3"/>
       <c r="O12" s="3"/>
-    </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="P12" s="3"/>
+    </row>
+    <row r="13" spans="1:18">
       <c r="C13" s="3"/>
       <c r="D13" s="3"/>
       <c r="E13" s="3"/>
@@ -856,8 +879,9 @@
       <c r="M13" s="3"/>
       <c r="N13" s="3"/>
       <c r="O13" s="3"/>
-    </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="P13" s="3"/>
+    </row>
+    <row r="14" spans="1:18">
       <c r="C14" s="3"/>
       <c r="D14" s="3"/>
       <c r="E14" s="3"/>
@@ -871,8 +895,9 @@
       <c r="M14" s="3"/>
       <c r="N14" s="3"/>
       <c r="O14" s="3"/>
-    </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="P14" s="3"/>
+    </row>
+    <row r="15" spans="1:18">
       <c r="C15" s="3"/>
       <c r="D15" s="3"/>
       <c r="E15" s="3"/>
@@ -886,6 +911,7 @@
       <c r="M15" s="3"/>
       <c r="N15" s="3"/>
       <c r="O15" s="3"/>
+      <c r="P15" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
KIBON-197 replace gesperrt flag with BenutzerStatus
</commit_message>
<xml_diff>
--- a/ebegu-server/src/main/resources/reporting/Benutzer.xlsx
+++ b/ebegu-server/src/main/resources/reporting/Benutzer.xlsx
@@ -1,16 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20829"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
-  <xr:revisionPtr revIDLastSave="3" documentId="11_80BED6E07095660F07BF7CE8808D0197A6985912" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{B6C82381-52D1-4A2F-9D62-B766F5AADA47}"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\Client\A$\IdeaProjects\ebegu\ebegu-server\src\main\resources\reporting\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="975" yWindow="360" windowWidth="28800" windowHeight="12435" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="975" yWindow="360" windowWidth="28800" windowHeight="12435"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="179020"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -79,9 +83,6 @@
     <t>Schulamt-Angebote</t>
   </si>
   <si>
-    <t>Gesperrt</t>
-  </si>
-  <si>
     <t>{username}</t>
   </si>
   <si>
@@ -130,17 +131,20 @@
     <t>{isSchulamt}</t>
   </si>
   <si>
-    <t>{gesperrt}</t>
-  </si>
-  <si>
     <t>{repeatBenutzerRow}</t>
+  </si>
+  <si>
+    <t>{status}</t>
+  </si>
+  <si>
+    <t>Status</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
-  <fonts count="3">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -279,7 +283,7 @@
     </dxf>
   </dxfs>
   <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
-    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2" xr9:uid="{00000000-0011-0000-FFFF-FFFF00000000}">
+    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2">
       <tableStyleElement type="wholeTable" dxfId="1"/>
       <tableStyleElement type="headerRow" dxfId="0"/>
     </tableStyle>
@@ -557,14 +561,12 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R15"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0" xr3:uid="{AEA406A1-0E4B-5B11-9CD5-51D6E497D94C}">
-      <selection activeCell="G6" sqref="G6"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="22.28515625" customWidth="1"/>
     <col min="2" max="2" width="22" customWidth="1"/>
@@ -584,7 +586,7 @@
     <col min="17" max="17" width="12.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" ht="21">
+    <row r="1" spans="1:18" ht="21" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -604,7 +606,7 @@
       <c r="O1" s="2"/>
       <c r="P1" s="2"/>
     </row>
-    <row r="2" spans="1:18">
+    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
       <c r="C2" s="3"/>
       <c r="D2" s="3"/>
       <c r="E2" s="3"/>
@@ -620,7 +622,7 @@
       <c r="O2" s="3"/>
       <c r="P2" s="3"/>
     </row>
-    <row r="3" spans="1:18">
+    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -642,7 +644,7 @@
       <c r="O3" s="5"/>
       <c r="P3" s="5"/>
     </row>
-    <row r="4" spans="1:18">
+    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
       <c r="C4" s="3"/>
       <c r="D4" s="3"/>
       <c r="E4" s="3"/>
@@ -658,7 +660,7 @@
       <c r="O4" s="3"/>
       <c r="P4" s="3"/>
     </row>
-    <row r="5" spans="1:18">
+    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A5" s="7" t="s">
         <v>3</v>
       </c>
@@ -708,66 +710,66 @@
         <v>18</v>
       </c>
       <c r="Q5" s="7" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A6" s="9" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="6" spans="1:18">
-      <c r="A6" s="9" t="s">
+      <c r="B6" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="B6" s="9" t="s">
+      <c r="C6" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="C6" s="9" t="s">
+      <c r="D6" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="D6" s="9" t="s">
+      <c r="E6" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="E6" s="9" t="s">
+      <c r="F6" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="F6" s="11" t="s">
+      <c r="G6" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="G6" s="11" t="s">
+      <c r="H6" s="9" t="s">
         <v>26</v>
       </c>
-      <c r="H6" s="9" t="s">
+      <c r="I6" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="I6" s="9" t="s">
+      <c r="J6" s="10" t="s">
         <v>28</v>
       </c>
-      <c r="J6" s="10" t="s">
+      <c r="K6" s="10" t="s">
         <v>29</v>
       </c>
-      <c r="K6" s="10" t="s">
+      <c r="L6" s="10" t="s">
         <v>30</v>
       </c>
-      <c r="L6" s="10" t="s">
+      <c r="M6" s="10" t="s">
         <v>31</v>
       </c>
-      <c r="M6" s="10" t="s">
+      <c r="N6" s="10" t="s">
         <v>32</v>
       </c>
-      <c r="N6" s="10" t="s">
+      <c r="O6" s="10" t="s">
         <v>33</v>
       </c>
-      <c r="O6" s="10" t="s">
+      <c r="P6" s="10" t="s">
         <v>34</v>
-      </c>
-      <c r="P6" s="10" t="s">
-        <v>35</v>
       </c>
       <c r="Q6" s="10" t="s">
         <v>36</v>
       </c>
       <c r="R6" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="7" spans="1:18">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
       <c r="C7" s="3"/>
       <c r="D7" s="3"/>
       <c r="E7" s="3"/>
@@ -783,7 +785,7 @@
       <c r="O7" s="3"/>
       <c r="P7" s="3"/>
     </row>
-    <row r="8" spans="1:18">
+    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A8" s="4"/>
       <c r="B8" s="4"/>
       <c r="C8" s="5"/>
@@ -801,7 +803,7 @@
       <c r="O8" s="5"/>
       <c r="P8" s="5"/>
     </row>
-    <row r="9" spans="1:18">
+    <row r="9" spans="1:18" x14ac:dyDescent="0.25">
       <c r="C9" s="3"/>
       <c r="D9" s="3"/>
       <c r="E9" s="3"/>
@@ -817,7 +819,7 @@
       <c r="O9" s="3"/>
       <c r="P9" s="3"/>
     </row>
-    <row r="10" spans="1:18">
+    <row r="10" spans="1:18" x14ac:dyDescent="0.25">
       <c r="C10" s="3"/>
       <c r="D10" s="3"/>
       <c r="E10" s="3"/>
@@ -833,7 +835,7 @@
       <c r="O10" s="3"/>
       <c r="P10" s="3"/>
     </row>
-    <row r="11" spans="1:18">
+    <row r="11" spans="1:18" x14ac:dyDescent="0.25">
       <c r="C11" s="3"/>
       <c r="D11" s="3"/>
       <c r="E11" s="3"/>
@@ -849,7 +851,7 @@
       <c r="O11" s="3"/>
       <c r="P11" s="3"/>
     </row>
-    <row r="12" spans="1:18">
+    <row r="12" spans="1:18" x14ac:dyDescent="0.25">
       <c r="C12" s="3"/>
       <c r="D12" s="3"/>
       <c r="E12" s="3"/>
@@ -865,7 +867,7 @@
       <c r="O12" s="3"/>
       <c r="P12" s="3"/>
     </row>
-    <row r="13" spans="1:18">
+    <row r="13" spans="1:18" x14ac:dyDescent="0.25">
       <c r="C13" s="3"/>
       <c r="D13" s="3"/>
       <c r="E13" s="3"/>
@@ -881,7 +883,7 @@
       <c r="O13" s="3"/>
       <c r="P13" s="3"/>
     </row>
-    <row r="14" spans="1:18">
+    <row r="14" spans="1:18" x14ac:dyDescent="0.25">
       <c r="C14" s="3"/>
       <c r="D14" s="3"/>
       <c r="E14" s="3"/>
@@ -897,7 +899,7 @@
       <c r="O14" s="3"/>
       <c r="P14" s="3"/>
     </row>
-    <row r="15" spans="1:18">
+    <row r="15" spans="1:18" x14ac:dyDescent="0.25">
       <c r="C15" s="3"/>
       <c r="D15" s="3"/>
       <c r="E15" s="3"/>

</xml_diff>

<commit_message>
KIBON-238: Tagi Code in einem Commit löschen
</commit_message>
<xml_diff>
--- a/ebegu-server/src/main/resources/reporting/Benutzer.xlsx
+++ b/ebegu-server/src/main/resources/reporting/Benutzer.xlsx
@@ -1,30 +1,36 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21009"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\Client\A$\IdeaProjects\ebegu\ebegu-server\src\main\resources\reporting\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{704528EE-8E86-496C-A44B-431973A65D97}" xr6:coauthVersionLast="39" xr6:coauthVersionMax="39" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="975" yWindow="360" windowWidth="28800" windowHeight="12435"/>
+    <workbookView xWindow="975" yWindow="360" windowWidth="28800" windowHeight="12435" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="179020"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="36">
   <si>
     <t>Benutzer</t>
   </si>
@@ -68,9 +74,6 @@
     <t>Tagesfamilien</t>
   </si>
   <si>
-    <t>Tagi</t>
-  </si>
-  <si>
     <t>Tagesschulen</t>
   </si>
   <si>
@@ -83,6 +86,9 @@
     <t>Schulamt-Angebote</t>
   </si>
   <si>
+    <t>Status</t>
+  </si>
+  <si>
     <t>{username}</t>
   </si>
   <si>
@@ -116,9 +122,6 @@
     <t>{isTagesfamilien}</t>
   </si>
   <si>
-    <t>{isTagi}</t>
-  </si>
-  <si>
     <t>{isTagesschule}</t>
   </si>
   <si>
@@ -131,20 +134,17 @@
     <t>{isSchulamt}</t>
   </si>
   <si>
+    <t>{status}</t>
+  </si>
+  <si>
     <t>{repeatBenutzerRow}</t>
-  </si>
-  <si>
-    <t>{status}</t>
-  </si>
-  <si>
-    <t>Status</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -283,7 +283,7 @@
     </dxf>
   </dxfs>
   <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
-    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2">
+    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2" xr9:uid="{00000000-0011-0000-FFFF-FFFF00000000}">
       <tableStyleElement type="wholeTable" dxfId="1"/>
       <tableStyleElement type="headerRow" dxfId="0"/>
     </tableStyle>
@@ -561,12 +561,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:R15"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:Q15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0" xr3:uid="{AEA406A1-0E4B-5B11-9CD5-51D6E497D94C}">
+      <selection activeCell="L1" sqref="L1:L1048576"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="22.28515625" customWidth="1"/>
     <col min="2" max="2" width="22" customWidth="1"/>
@@ -578,15 +580,14 @@
     <col min="9" max="9" width="28.7109375" customWidth="1"/>
     <col min="10" max="10" width="7.28515625" customWidth="1"/>
     <col min="11" max="11" width="16.42578125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="7.42578125" customWidth="1"/>
-    <col min="13" max="13" width="14.5703125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="13.85546875" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="20.28515625" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="18.7109375" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="12.28515625" customWidth="1"/>
+    <col min="12" max="12" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="20.28515625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="18.7109375" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="12.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" ht="21" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:17" ht="21">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -604,9 +605,8 @@
       <c r="M1" s="2"/>
       <c r="N1" s="2"/>
       <c r="O1" s="2"/>
-      <c r="P1" s="2"/>
-    </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:17">
       <c r="C2" s="3"/>
       <c r="D2" s="3"/>
       <c r="E2" s="3"/>
@@ -620,9 +620,8 @@
       <c r="M2" s="3"/>
       <c r="N2" s="3"/>
       <c r="O2" s="3"/>
-      <c r="P2" s="3"/>
-    </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
+    </row>
+    <row r="3" spans="1:17">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -642,9 +641,8 @@
       <c r="M3" s="5"/>
       <c r="N3" s="5"/>
       <c r="O3" s="5"/>
-      <c r="P3" s="5"/>
-    </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
+    </row>
+    <row r="4" spans="1:17">
       <c r="C4" s="3"/>
       <c r="D4" s="3"/>
       <c r="E4" s="3"/>
@@ -658,9 +656,8 @@
       <c r="M4" s="3"/>
       <c r="N4" s="3"/>
       <c r="O4" s="3"/>
-      <c r="P4" s="3"/>
-    </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
+    </row>
+    <row r="5" spans="1:17">
       <c r="A5" s="7" t="s">
         <v>3</v>
       </c>
@@ -706,14 +703,11 @@
       <c r="O5" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="P5" s="8" t="s">
+      <c r="P5" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="Q5" s="7" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
+    </row>
+    <row r="6" spans="1:17">
       <c r="A6" s="9" t="s">
         <v>19</v>
       </c>
@@ -762,14 +756,11 @@
       <c r="P6" s="10" t="s">
         <v>34</v>
       </c>
-      <c r="Q6" s="10" t="s">
-        <v>36</v>
-      </c>
-      <c r="R6" t="s">
+      <c r="Q6" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:17">
       <c r="C7" s="3"/>
       <c r="D7" s="3"/>
       <c r="E7" s="3"/>
@@ -783,9 +774,8 @@
       <c r="M7" s="3"/>
       <c r="N7" s="3"/>
       <c r="O7" s="3"/>
-      <c r="P7" s="3"/>
-    </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
+    </row>
+    <row r="8" spans="1:17">
       <c r="A8" s="4"/>
       <c r="B8" s="4"/>
       <c r="C8" s="5"/>
@@ -801,9 +791,8 @@
       <c r="M8" s="5"/>
       <c r="N8" s="5"/>
       <c r="O8" s="5"/>
-      <c r="P8" s="5"/>
-    </row>
-    <row r="9" spans="1:18" x14ac:dyDescent="0.25">
+    </row>
+    <row r="9" spans="1:17">
       <c r="C9" s="3"/>
       <c r="D9" s="3"/>
       <c r="E9" s="3"/>
@@ -817,9 +806,8 @@
       <c r="M9" s="3"/>
       <c r="N9" s="3"/>
       <c r="O9" s="3"/>
-      <c r="P9" s="3"/>
-    </row>
-    <row r="10" spans="1:18" x14ac:dyDescent="0.25">
+    </row>
+    <row r="10" spans="1:17">
       <c r="C10" s="3"/>
       <c r="D10" s="3"/>
       <c r="E10" s="3"/>
@@ -833,9 +821,8 @@
       <c r="M10" s="3"/>
       <c r="N10" s="3"/>
       <c r="O10" s="3"/>
-      <c r="P10" s="3"/>
-    </row>
-    <row r="11" spans="1:18" x14ac:dyDescent="0.25">
+    </row>
+    <row r="11" spans="1:17">
       <c r="C11" s="3"/>
       <c r="D11" s="3"/>
       <c r="E11" s="3"/>
@@ -849,9 +836,8 @@
       <c r="M11" s="3"/>
       <c r="N11" s="3"/>
       <c r="O11" s="3"/>
-      <c r="P11" s="3"/>
-    </row>
-    <row r="12" spans="1:18" x14ac:dyDescent="0.25">
+    </row>
+    <row r="12" spans="1:17">
       <c r="C12" s="3"/>
       <c r="D12" s="3"/>
       <c r="E12" s="3"/>
@@ -865,9 +851,8 @@
       <c r="M12" s="3"/>
       <c r="N12" s="3"/>
       <c r="O12" s="3"/>
-      <c r="P12" s="3"/>
-    </row>
-    <row r="13" spans="1:18" x14ac:dyDescent="0.25">
+    </row>
+    <row r="13" spans="1:17">
       <c r="C13" s="3"/>
       <c r="D13" s="3"/>
       <c r="E13" s="3"/>
@@ -881,9 +866,8 @@
       <c r="M13" s="3"/>
       <c r="N13" s="3"/>
       <c r="O13" s="3"/>
-      <c r="P13" s="3"/>
-    </row>
-    <row r="14" spans="1:18" x14ac:dyDescent="0.25">
+    </row>
+    <row r="14" spans="1:17">
       <c r="C14" s="3"/>
       <c r="D14" s="3"/>
       <c r="E14" s="3"/>
@@ -897,9 +881,8 @@
       <c r="M14" s="3"/>
       <c r="N14" s="3"/>
       <c r="O14" s="3"/>
-      <c r="P14" s="3"/>
-    </row>
-    <row r="15" spans="1:18" x14ac:dyDescent="0.25">
+    </row>
+    <row r="15" spans="1:17">
       <c r="C15" s="3"/>
       <c r="D15" s="3"/>
       <c r="E15" s="3"/>
@@ -913,7 +896,6 @@
       <c r="M15" s="3"/>
       <c r="N15" s="3"/>
       <c r="O15" s="3"/>
-      <c r="P15" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
KIBON-120: Benutzer statistik - We cannot directly use the LocaleThreadLocal in ReportServiceBean because it runs asynchronously and the value got lost. We need to use the language saved in the corresponding workjob - In this commit only the benutzer statistik was done. All other statistic will be done in future commits
</commit_message>
<xml_diff>
--- a/ebegu-server/src/main/resources/reporting/Benutzer.xlsx
+++ b/ebegu-server/src/main/resources/reporting/Benutzer.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21009"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21126"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\Client\A$\IdeaProjects\ebegu\ebegu-server\src\main\resources\reporting\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\Client\A$\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{704528EE-8E86-496C-A44B-431973A65D97}" xr6:coauthVersionLast="39" xr6:coauthVersionMax="39" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C91454DD-6425-4F83-8AB4-1A944B81422C}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="975" yWindow="360" windowWidth="28800" windowHeight="12435" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -32,63 +32,9 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="36">
   <si>
-    <t>Benutzer</t>
-  </si>
-  <si>
-    <t>Stichtag</t>
-  </si>
-  <si>
     <t>{stichtag}</t>
   </si>
   <si>
-    <t>Username</t>
-  </si>
-  <si>
-    <t>Vorname</t>
-  </si>
-  <si>
-    <t>Nachname</t>
-  </si>
-  <si>
-    <t>E-Mail</t>
-  </si>
-  <si>
-    <t>Rolle</t>
-  </si>
-  <si>
-    <t>Rolle gültig bis</t>
-  </si>
-  <si>
-    <t>Gemeinde(n)</t>
-  </si>
-  <si>
-    <t>Institution</t>
-  </si>
-  <si>
-    <t>Trägerschaft</t>
-  </si>
-  <si>
-    <t>Kita</t>
-  </si>
-  <si>
-    <t>Tagesfamilien</t>
-  </si>
-  <si>
-    <t>Tagesschulen</t>
-  </si>
-  <si>
-    <t>Ferieninsel</t>
-  </si>
-  <si>
-    <t>Jugendamt-Angebote</t>
-  </si>
-  <si>
-    <t>Schulamt-Angebote</t>
-  </si>
-  <si>
-    <t>Status</t>
-  </si>
-  <si>
     <t>{username}</t>
   </si>
   <si>
@@ -138,13 +84,67 @@
   </si>
   <si>
     <t>{repeatBenutzerRow}</t>
+  </si>
+  <si>
+    <t>{usernameTitle}</t>
+  </si>
+  <si>
+    <t>{vornameTitle}</t>
+  </si>
+  <si>
+    <t>{nachnameTitle}</t>
+  </si>
+  <si>
+    <t>{emailTitle}</t>
+  </si>
+  <si>
+    <t>{roleTitle}</t>
+  </si>
+  <si>
+    <t>{roleGueltigBisTitel}</t>
+  </si>
+  <si>
+    <t>{gemeindenTitle}</t>
+  </si>
+  <si>
+    <t>{institutionTitle}</t>
+  </si>
+  <si>
+    <t>{traegerschaftTitle}</t>
+  </si>
+  <si>
+    <t>{kitaTitel}</t>
+  </si>
+  <si>
+    <t>{tagesfamilienTitle}</t>
+  </si>
+  <si>
+    <t>{tagesschulenTitel}</t>
+  </si>
+  <si>
+    <t>{ferieninselTitle}</t>
+  </si>
+  <si>
+    <t>{isSchulamtTitle}</t>
+  </si>
+  <si>
+    <t>{isJugendamtTitle}</t>
+  </si>
+  <si>
+    <t>{statusTitle}</t>
+  </si>
+  <si>
+    <t>{stichtagTitle}</t>
+  </si>
+  <si>
+    <t>{reportBenutzerTitle}</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
-  <fonts count="3">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -564,21 +564,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Q15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0" xr3:uid="{AEA406A1-0E4B-5B11-9CD5-51D6E497D94C}">
-      <selection activeCell="L1" sqref="L1:L1048576"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="22.28515625" customWidth="1"/>
     <col min="2" max="2" width="22" customWidth="1"/>
     <col min="3" max="3" width="21" customWidth="1"/>
     <col min="4" max="4" width="36" customWidth="1"/>
     <col min="5" max="5" width="33.7109375" customWidth="1"/>
-    <col min="6" max="7" width="16.5703125" customWidth="1"/>
+    <col min="6" max="6" width="16.85546875" customWidth="1"/>
+    <col min="7" max="7" width="16.5703125" customWidth="1"/>
     <col min="8" max="8" width="30.140625" customWidth="1"/>
     <col min="9" max="9" width="28.7109375" customWidth="1"/>
-    <col min="10" max="10" width="7.28515625" customWidth="1"/>
+    <col min="10" max="10" width="13.42578125" customWidth="1"/>
     <col min="11" max="11" width="16.42578125" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="14.5703125" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="13.85546875" bestFit="1" customWidth="1"/>
@@ -587,9 +586,9 @@
     <col min="16" max="16" width="12.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" ht="21">
+    <row r="1" spans="1:17" ht="21" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
-        <v>0</v>
+        <v>35</v>
       </c>
       <c r="B1" s="1"/>
       <c r="C1" s="2"/>
@@ -606,7 +605,7 @@
       <c r="N1" s="2"/>
       <c r="O1" s="2"/>
     </row>
-    <row r="2" spans="1:17">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
       <c r="C2" s="3"/>
       <c r="D2" s="3"/>
       <c r="E2" s="3"/>
@@ -621,12 +620,12 @@
       <c r="N2" s="3"/>
       <c r="O2" s="3"/>
     </row>
-    <row r="3" spans="1:17">
+    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>1</v>
+        <v>34</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="C3" s="5"/>
       <c r="D3" s="5"/>
@@ -642,7 +641,7 @@
       <c r="N3" s="5"/>
       <c r="O3" s="5"/>
     </row>
-    <row r="4" spans="1:17">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
       <c r="C4" s="3"/>
       <c r="D4" s="3"/>
       <c r="E4" s="3"/>
@@ -657,110 +656,110 @@
       <c r="N4" s="3"/>
       <c r="O4" s="3"/>
     </row>
-    <row r="5" spans="1:17">
+    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A5" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="B5" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="C5" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="D5" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="E5" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="F5" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="G5" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="H5" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="I5" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="J5" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="K5" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="L5" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="M5" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="N5" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="O5" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="P5" s="7" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A6" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="B6" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="C6" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="7" t="s">
+      <c r="D6" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="C5" s="8" t="s">
+      <c r="E6" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="D5" s="8" t="s">
+      <c r="F6" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="E5" s="8" t="s">
+      <c r="G6" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="F5" s="8" t="s">
+      <c r="H6" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="G5" s="8" t="s">
+      <c r="I6" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="H5" s="8" t="s">
+      <c r="J6" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="I5" s="8" t="s">
+      <c r="K6" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="J5" s="8" t="s">
+      <c r="L6" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="K5" s="8" t="s">
+      <c r="M6" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="L5" s="8" t="s">
+      <c r="N6" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="M5" s="8" t="s">
+      <c r="O6" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="N5" s="8" t="s">
+      <c r="P6" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="O5" s="8" t="s">
+      <c r="Q6" t="s">
         <v>17</v>
       </c>
-      <c r="P5" s="7" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="6" spans="1:17">
-      <c r="A6" s="9" t="s">
-        <v>19</v>
-      </c>
-      <c r="B6" s="9" t="s">
-        <v>20</v>
-      </c>
-      <c r="C6" s="9" t="s">
-        <v>21</v>
-      </c>
-      <c r="D6" s="9" t="s">
-        <v>22</v>
-      </c>
-      <c r="E6" s="9" t="s">
-        <v>23</v>
-      </c>
-      <c r="F6" s="11" t="s">
-        <v>24</v>
-      </c>
-      <c r="G6" s="11" t="s">
-        <v>25</v>
-      </c>
-      <c r="H6" s="9" t="s">
-        <v>26</v>
-      </c>
-      <c r="I6" s="9" t="s">
-        <v>27</v>
-      </c>
-      <c r="J6" s="10" t="s">
-        <v>28</v>
-      </c>
-      <c r="K6" s="10" t="s">
-        <v>29</v>
-      </c>
-      <c r="L6" s="10" t="s">
-        <v>30</v>
-      </c>
-      <c r="M6" s="10" t="s">
-        <v>31</v>
-      </c>
-      <c r="N6" s="10" t="s">
-        <v>32</v>
-      </c>
-      <c r="O6" s="10" t="s">
-        <v>33</v>
-      </c>
-      <c r="P6" s="10" t="s">
-        <v>34</v>
-      </c>
-      <c r="Q6" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="7" spans="1:17">
+    </row>
+    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
       <c r="C7" s="3"/>
       <c r="D7" s="3"/>
       <c r="E7" s="3"/>
@@ -775,7 +774,7 @@
       <c r="N7" s="3"/>
       <c r="O7" s="3"/>
     </row>
-    <row r="8" spans="1:17">
+    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A8" s="4"/>
       <c r="B8" s="4"/>
       <c r="C8" s="5"/>
@@ -792,7 +791,7 @@
       <c r="N8" s="5"/>
       <c r="O8" s="5"/>
     </row>
-    <row r="9" spans="1:17">
+    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
       <c r="C9" s="3"/>
       <c r="D9" s="3"/>
       <c r="E9" s="3"/>
@@ -807,7 +806,7 @@
       <c r="N9" s="3"/>
       <c r="O9" s="3"/>
     </row>
-    <row r="10" spans="1:17">
+    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
       <c r="C10" s="3"/>
       <c r="D10" s="3"/>
       <c r="E10" s="3"/>
@@ -822,7 +821,7 @@
       <c r="N10" s="3"/>
       <c r="O10" s="3"/>
     </row>
-    <row r="11" spans="1:17">
+    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
       <c r="C11" s="3"/>
       <c r="D11" s="3"/>
       <c r="E11" s="3"/>
@@ -837,7 +836,7 @@
       <c r="N11" s="3"/>
       <c r="O11" s="3"/>
     </row>
-    <row r="12" spans="1:17">
+    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
       <c r="C12" s="3"/>
       <c r="D12" s="3"/>
       <c r="E12" s="3"/>
@@ -852,7 +851,7 @@
       <c r="N12" s="3"/>
       <c r="O12" s="3"/>
     </row>
-    <row r="13" spans="1:17">
+    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
       <c r="C13" s="3"/>
       <c r="D13" s="3"/>
       <c r="E13" s="3"/>
@@ -867,7 +866,7 @@
       <c r="N13" s="3"/>
       <c r="O13" s="3"/>
     </row>
-    <row r="14" spans="1:17">
+    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
       <c r="C14" s="3"/>
       <c r="D14" s="3"/>
       <c r="E14" s="3"/>
@@ -882,7 +881,7 @@
       <c r="N14" s="3"/>
       <c r="O14" s="3"/>
     </row>
-    <row r="15" spans="1:17">
+    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
       <c r="C15" s="3"/>
       <c r="D15" s="3"/>
       <c r="E15" s="3"/>

</xml_diff>

<commit_message>
KIBON-120: Column Gemeinde added for all Statistics that need it
</commit_message>
<xml_diff>
--- a/ebegu-server/src/main/resources/reporting/Benutzer.xlsx
+++ b/ebegu-server/src/main/resources/reporting/Benutzer.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21126"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\Client\A$\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\reporting_new\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C91454DD-6425-4F83-8AB4-1A944B81422C}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="975" yWindow="360" windowWidth="28800" windowHeight="12435" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="972" yWindow="360" windowWidth="28800" windowHeight="12432"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="1" r:id="rId1"/>
@@ -143,7 +142,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -283,7 +282,7 @@
     </dxf>
   </dxfs>
   <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
-    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2" xr9:uid="{00000000-0011-0000-FFFF-FFFF00000000}">
+    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2">
       <tableStyleElement type="wholeTable" dxfId="1"/>
       <tableStyleElement type="headerRow" dxfId="0"/>
     </tableStyle>
@@ -561,32 +560,34 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="22.28515625" customWidth="1"/>
+    <col min="1" max="1" width="22.33203125" customWidth="1"/>
     <col min="2" max="2" width="22" customWidth="1"/>
     <col min="3" max="3" width="21" customWidth="1"/>
     <col min="4" max="4" width="36" customWidth="1"/>
-    <col min="5" max="5" width="33.7109375" customWidth="1"/>
-    <col min="6" max="6" width="16.85546875" customWidth="1"/>
-    <col min="7" max="7" width="16.5703125" customWidth="1"/>
-    <col min="8" max="8" width="30.140625" customWidth="1"/>
-    <col min="9" max="9" width="28.7109375" customWidth="1"/>
-    <col min="10" max="10" width="13.42578125" customWidth="1"/>
-    <col min="11" max="11" width="16.42578125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="14.5703125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="13.85546875" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="20.28515625" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="18.7109375" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="12.28515625" customWidth="1"/>
+    <col min="5" max="5" width="33.6640625" customWidth="1"/>
+    <col min="6" max="6" width="16.88671875" customWidth="1"/>
+    <col min="7" max="7" width="16.5546875" customWidth="1"/>
+    <col min="8" max="8" width="30.109375" customWidth="1"/>
+    <col min="9" max="9" width="28.6640625" customWidth="1"/>
+    <col min="10" max="10" width="13.44140625" customWidth="1"/>
+    <col min="11" max="11" width="16.44140625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="14.5546875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="13.88671875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="20.33203125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="18.6640625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="12.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" ht="21" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:17" ht="21" x14ac:dyDescent="0.4">
       <c r="A1" s="1" t="s">
         <v>35</v>
       </c>
@@ -605,7 +606,7 @@
       <c r="N1" s="2"/>
       <c r="O1" s="2"/>
     </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.3">
       <c r="C2" s="3"/>
       <c r="D2" s="3"/>
       <c r="E2" s="3"/>
@@ -620,7 +621,7 @@
       <c r="N2" s="3"/>
       <c r="O2" s="3"/>
     </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>34</v>
       </c>
@@ -641,7 +642,7 @@
       <c r="N3" s="5"/>
       <c r="O3" s="5"/>
     </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.3">
       <c r="C4" s="3"/>
       <c r="D4" s="3"/>
       <c r="E4" s="3"/>
@@ -656,7 +657,7 @@
       <c r="N4" s="3"/>
       <c r="O4" s="3"/>
     </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A5" s="7" t="s">
         <v>18</v>
       </c>
@@ -706,7 +707,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A6" s="9" t="s">
         <v>1</v>
       </c>
@@ -759,7 +760,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:17" x14ac:dyDescent="0.3">
       <c r="C7" s="3"/>
       <c r="D7" s="3"/>
       <c r="E7" s="3"/>
@@ -774,7 +775,7 @@
       <c r="N7" s="3"/>
       <c r="O7" s="3"/>
     </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A8" s="4"/>
       <c r="B8" s="4"/>
       <c r="C8" s="5"/>
@@ -791,7 +792,7 @@
       <c r="N8" s="5"/>
       <c r="O8" s="5"/>
     </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:17" x14ac:dyDescent="0.3">
       <c r="C9" s="3"/>
       <c r="D9" s="3"/>
       <c r="E9" s="3"/>
@@ -806,7 +807,7 @@
       <c r="N9" s="3"/>
       <c r="O9" s="3"/>
     </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:17" x14ac:dyDescent="0.3">
       <c r="C10" s="3"/>
       <c r="D10" s="3"/>
       <c r="E10" s="3"/>
@@ -821,7 +822,7 @@
       <c r="N10" s="3"/>
       <c r="O10" s="3"/>
     </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:17" x14ac:dyDescent="0.3">
       <c r="C11" s="3"/>
       <c r="D11" s="3"/>
       <c r="E11" s="3"/>
@@ -836,7 +837,7 @@
       <c r="N11" s="3"/>
       <c r="O11" s="3"/>
     </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:17" x14ac:dyDescent="0.3">
       <c r="C12" s="3"/>
       <c r="D12" s="3"/>
       <c r="E12" s="3"/>
@@ -851,7 +852,7 @@
       <c r="N12" s="3"/>
       <c r="O12" s="3"/>
     </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:17" x14ac:dyDescent="0.3">
       <c r="C13" s="3"/>
       <c r="D13" s="3"/>
       <c r="E13" s="3"/>
@@ -866,7 +867,7 @@
       <c r="N13" s="3"/>
       <c r="O13" s="3"/>
     </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:17" x14ac:dyDescent="0.3">
       <c r="C14" s="3"/>
       <c r="D14" s="3"/>
       <c r="E14" s="3"/>
@@ -881,7 +882,7 @@
       <c r="N14" s="3"/>
       <c r="O14" s="3"/>
     </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:17" x14ac:dyDescent="0.3">
       <c r="C15" s="3"/>
       <c r="D15" s="3"/>
       <c r="E15" s="3"/>

</xml_diff>

<commit_message>
KIBON-1758 add angebotGemeinden to excel template and converter
</commit_message>
<xml_diff>
--- a/ebegu-server/src/main/resources/reporting/Benutzer.xlsx
+++ b/ebegu-server/src/main/resources/reporting/Benutzer.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23628"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\reporting_new\new\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\enja\IdeaProjects\ebegu\ebegu-server\src\main\resources\reporting\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{64018579-0B0F-4817-A02E-18243BF19ED7}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6DE265A3-A8BA-4D8B-8936-2DC1E86DA885}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="13965" xr2:uid="{617232BA-F9C5-4529-BA67-503720E5A6AB}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{617232BA-F9C5-4529-BA67-503720E5A6AB}"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="38">
   <si>
     <t>{reportBenutzerTitle}</t>
   </si>
@@ -139,6 +139,12 @@
   </si>
   <si>
     <t>{repeatBenutzerRow}</t>
+  </si>
+  <si>
+    <t>{angebotGemeindenTitle}</t>
+  </si>
+  <si>
+    <t>{angebotGemeinden}</t>
   </si>
 </sst>
 </file>
@@ -539,11 +545,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{42B88504-77C9-47C6-9364-CB212A99C694}">
-  <dimension ref="A1:Q6"/>
+  <dimension ref="A1:R6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -554,22 +558,23 @@
     <col min="5" max="5" width="32.85546875" customWidth="1"/>
     <col min="6" max="6" width="20" customWidth="1"/>
     <col min="7" max="7" width="22" customWidth="1"/>
-    <col min="8" max="8" width="28.85546875" customWidth="1"/>
-    <col min="9" max="9" width="28" customWidth="1"/>
-    <col min="10" max="10" width="14.5703125" customWidth="1"/>
-    <col min="11" max="11" width="18.5703125" customWidth="1"/>
-    <col min="12" max="12" width="21.42578125" customWidth="1"/>
-    <col min="13" max="13" width="21.85546875" customWidth="1"/>
-    <col min="14" max="14" width="20.5703125" customWidth="1"/>
-    <col min="15" max="15" width="17.85546875" customWidth="1"/>
+    <col min="8" max="8" width="22.85546875" customWidth="1"/>
+    <col min="9" max="9" width="28.85546875" customWidth="1"/>
+    <col min="10" max="10" width="28" customWidth="1"/>
+    <col min="11" max="11" width="14.5703125" customWidth="1"/>
+    <col min="12" max="12" width="18.5703125" customWidth="1"/>
+    <col min="13" max="13" width="21.42578125" customWidth="1"/>
+    <col min="14" max="14" width="21.85546875" customWidth="1"/>
+    <col min="15" max="15" width="20.5703125" customWidth="1"/>
+    <col min="16" max="16" width="17.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" ht="21" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:18" ht="21" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -577,7 +582,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
         <v>3</v>
       </c>
@@ -600,34 +605,37 @@
         <v>15</v>
       </c>
       <c r="H5" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="I5" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="I5" s="6" t="s">
+      <c r="J5" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="J5" s="6" t="s">
+      <c r="K5" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="K5" s="6" t="s">
+      <c r="L5" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="L5" s="6" t="s">
+      <c r="M5" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="M5" s="6" t="s">
+      <c r="N5" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="N5" s="6" t="s">
+      <c r="O5" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="O5" s="6" t="s">
+      <c r="P5" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="P5" s="6" t="s">
+      <c r="Q5" s="6" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>4</v>
       </c>
@@ -650,33 +658,36 @@
         <v>16</v>
       </c>
       <c r="H6" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="I6" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="I6" s="3" t="s">
+      <c r="J6" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="J6" s="4" t="s">
+      <c r="K6" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="K6" s="5" t="s">
+      <c r="L6" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="L6" s="5" t="s">
+      <c r="M6" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="M6" s="5" t="s">
+      <c r="N6" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="N6" s="5" t="s">
+      <c r="O6" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="O6" s="5" t="s">
+      <c r="P6" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="P6" s="3" t="s">
+      <c r="Q6" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="Q6" s="2" t="s">
+      <c r="R6" s="2" t="s">
         <v>35</v>
       </c>
     </row>

</xml_diff>